<commit_message>
Worked on modulating script
</commit_message>
<xml_diff>
--- a/clan/aphasiaComparisons.xlsx
+++ b/clan/aphasiaComparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr date1904="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jskne\Desktop\IMMERSE-2025\aphasia-analysis\clan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6D710B6A-940B-4328-9D4B-AF4DFCF3E514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C31BEA-BE0E-489D-AB50-91D3DAEAD8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{F70E3DF1-7393-4AA2-A4A4-C7D173FC07F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F70E3DF1-7393-4AA2-A4A4-C7D173FC07F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="111">
   <si>
     <t>File</t>
   </si>
@@ -309,13 +309,73 @@
   </si>
   <si>
     <t>generic1</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>62;06.</t>
+  </si>
+  <si>
+    <t>NEURAL</t>
+  </si>
+  <si>
+    <t>neural15-2Control.cha</t>
+  </si>
+  <si>
+    <t>MSU</t>
+  </si>
+  <si>
+    <t>msu08aControl.cha</t>
+  </si>
+  <si>
+    <t>48;01.</t>
+  </si>
+  <si>
+    <t>msu07aControl.cha</t>
+  </si>
+  <si>
+    <t>75;07.</t>
+  </si>
+  <si>
+    <t>Kempler</t>
+  </si>
+  <si>
+    <t>kempler01Control.cha</t>
+  </si>
+  <si>
+    <t>82;04.</t>
+  </si>
+  <si>
+    <t>Capilouto</t>
+  </si>
+  <si>
+    <t>capilouto06Control.cha</t>
+  </si>
+  <si>
+    <t>72;03.</t>
+  </si>
+  <si>
+    <t>capilouto05Control.cha</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>generic2</t>
+  </si>
+  <si>
+    <t>generic3</t>
+  </si>
+  <si>
+    <t>generic4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +510,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +697,24 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -792,8 +876,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,783 +974,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Broca's</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs Wernicke's vs Generic Prompt Averages</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.8872828929612356E-2"/>
-          <c:y val="0.10000673019946656"/>
-          <c:w val="0.92898264793685692"/>
-          <c:h val="0.77598010918209392"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Main!$M$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Broca Avg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Main!$X$1:$AT$1</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>density</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>%_Nouns</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>%_Plurals</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>%_Verbs</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>%_Aux</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>%_Mod</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>%_3S</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>%_13S</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>%_PAST</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>%_PASTP</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>%_PRESP</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>%_prep</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>%_adj</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>%_adv</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>%_conj</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>%_det</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>%_pro</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>noun_verb</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>open_closed</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Main!$X$13:$AT$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0.25339999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.954399999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.714599999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.9987999999999992</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.57940000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.034</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>25.308799999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1960000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.0468000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.6348000000000003</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.526599999999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.55579999999999996</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.6411999999999995</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.0304000000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.5728</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.1929999999999996</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.9698000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.2902</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.62419999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD82-4B4E-A0B9-5F72BB1CAB17}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Main!$M$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Wernicke Avg.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Main!$X$1:$AT$1</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>density</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>%_Nouns</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>%_Plurals</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>%_Verbs</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>%_Aux</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>%_Mod</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>%_3S</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>%_13S</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>%_PAST</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>%_PASTP</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>%_PRESP</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>%_prep</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>%_adj</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>%_adv</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>%_conj</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>%_det</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>%_pro</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>noun_verb</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>open_closed</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Main!$X$14:$AT$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0.39039999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.8979999999999997</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23.019799999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16.685200000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.8502000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9543999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>24.341999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.6912000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>21.927799999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.8537999999999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20.641999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.4601999999999995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.0900000000000003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.0136000000000003</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6707999999999998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.3980000000000006</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18.477</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.53900000000000003</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.5643999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FD82-4B4E-A0B9-5F72BB1CAB17}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Main!$M$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Generic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Main!$X$1:$AT$1</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>density</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>%_Nouns</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>%_Plurals</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>%_Verbs</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>%_Aux</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>%_Mod</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>%_3S</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>%_13S</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>%_PAST</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>%_PASTP</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>%_PRESP</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>%_prep</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>%_adj</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>%_adv</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>%_conj</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>%_det</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>%_pro</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>noun_verb</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>open_closed</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Main!$X$15:$AT$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.373</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>53.726999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1789999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.839</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.77600000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>27.451000000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.706</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.9220000000000002</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11.765000000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.0369999999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.9009999999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.9189999999999996</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.155</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.0190000000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.8820000000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.3919999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000022-FD82-4B4E-A0B9-5F72BB1CAB17}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="363954336"/>
-        <c:axId val="363959616"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="363954336"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="363959616"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="363959616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="363954336"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Broca</a:t>
             </a:r>
             <a:r>
@@ -1713,7 +1023,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.5585183623072662E-2"/>
+          <c:y val="8.6711538461538479E-2"/>
+          <c:w val="0.9635881985002418"/>
+          <c:h val="0.8402242580254391"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1723,7 +1043,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Main!$M$13</c:f>
+              <c:f>Main!$M$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1782,7 +1102,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Main!$N$13:$W$13</c:f>
+              <c:f>Main!$N$27:$W$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1830,7 +1150,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Main!$M$14</c:f>
+              <c:f>Main!$M$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1889,7 +1209,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Main!$N$14:$W$14</c:f>
+              <c:f>Main!$N$28:$W$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1937,7 +1257,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Main!$M$15</c:f>
+              <c:f>Main!$M$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1996,7 +1316,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Main!$N$15:$W$15</c:f>
+              <c:f>Main!$N$29:$W$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2036,6 +1356,187 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0884-4256-AC53-508B3B56D25C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$M$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Control</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$N$1:$W$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Total_Utts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MLU_Utts</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLU_Words</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MLU_Morphemes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FREQ_types</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FREQ_tokens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FREQ_TTR</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Verbs_Utt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>%_Word_Errors</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Utt_Errors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$N$30:$W$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>161.83333333333334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>161.83333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6994999999999987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.527499999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>399.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1574.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27550000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6696666666666669</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5666666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8333333333333335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BBB6-4A5F-BDB5-6CDBDB3F5B81}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$M$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Main!$N$1:$W$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Total_Utts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MLU_Utts</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MLU_Words</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MLU_Morphemes</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>FREQ_types</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FREQ_tokens</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FREQ_TTR</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Verbs_Utt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>%_Word_Errors</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Utt_Errors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Main!$N$31:$W$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BBB6-4A5F-BDB5-6CDBDB3F5B81}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2243,46 +1744,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2825,559 +2286,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>20956</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>60004</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>10660</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>99059</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BA80CF-5601-3146-7338-FEA798998F36}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>26669</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>1905</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>59765</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3396,7 +2318,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3722,19 +2644,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC29546-9928-44F8-BA92-163A393956D5}">
-  <dimension ref="A1:AT15"/>
+  <dimension ref="A1:AT30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I49" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="46" width="0" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="10.6640625" customWidth="1"/>
+    <col min="44" max="44" width="10" customWidth="1"/>
+    <col min="45" max="45" width="6.77734375" customWidth="1"/>
+    <col min="46" max="46" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" ht="15" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3874,8 +2799,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:46" ht="15" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B2" t="s">
@@ -4014,8 +2939,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:46" ht="15" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B3" t="s">
@@ -4154,8 +3079,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:46" ht="15" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B4" t="s">
@@ -4294,8 +3219,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:46" ht="15" customHeight="1">
+      <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B5" t="s">
@@ -4434,8 +3359,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:46" ht="15" customHeight="1">
+      <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B6" t="s">
@@ -4574,8 +3499,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:46" ht="15" customHeight="1">
+      <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
@@ -4714,8 +3639,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:46" ht="15" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
@@ -4854,8 +3779,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:46" ht="15" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B9" t="s">
@@ -4994,8 +3919,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:46" ht="15" customHeight="1">
+      <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B10" t="s">
@@ -5134,8 +4059,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:46" ht="15" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B11" t="s">
@@ -5274,8 +4199,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:46" ht="15" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G12" t="s">
@@ -5384,399 +4309,1363 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M13" t="s">
+    <row r="13" spans="1:46" ht="15" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:46" ht="15" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:46" ht="15" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" ht="15" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>123</v>
+      </c>
+      <c r="O16">
+        <v>123</v>
+      </c>
+      <c r="P16">
+        <v>10.707000000000001</v>
+      </c>
+      <c r="Q16">
+        <v>11.691000000000001</v>
+      </c>
+      <c r="R16">
+        <v>421</v>
+      </c>
+      <c r="S16">
+        <v>1334</v>
+      </c>
+      <c r="T16">
+        <v>0.316</v>
+      </c>
+      <c r="U16">
+        <v>1.6830000000000001</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0.49</v>
+      </c>
+      <c r="Y16">
+        <v>19.864999999999998</v>
+      </c>
+      <c r="Z16">
+        <v>14.34</v>
+      </c>
+      <c r="AA16">
+        <v>17.091000000000001</v>
+      </c>
+      <c r="AB16">
+        <v>2.774</v>
+      </c>
+      <c r="AC16">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="AD16">
+        <v>24.123000000000001</v>
+      </c>
+      <c r="AE16">
+        <v>6.14</v>
+      </c>
+      <c r="AF16">
+        <v>35.526000000000003</v>
+      </c>
+      <c r="AG16">
+        <v>12.281000000000001</v>
+      </c>
+      <c r="AH16">
+        <v>14.474</v>
+      </c>
+      <c r="AI16">
+        <v>8.1709999999999994</v>
+      </c>
+      <c r="AJ16">
+        <v>5.0970000000000004</v>
+      </c>
+      <c r="AK16">
+        <v>5.7720000000000002</v>
+      </c>
+      <c r="AL16">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="AM16">
+        <v>10.795</v>
+      </c>
+      <c r="AN16">
+        <v>11.468999999999999</v>
+      </c>
+      <c r="AO16">
+        <v>1.1619999999999999</v>
+      </c>
+      <c r="AP16">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="AQ16">
+        <v>638</v>
+      </c>
+      <c r="AR16">
+        <v>684</v>
+      </c>
+      <c r="AS16">
+        <v>13</v>
+      </c>
+      <c r="AT16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" ht="15" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" t="s">
+        <v>51</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>191</v>
+      </c>
+      <c r="O17">
+        <v>191</v>
+      </c>
+      <c r="P17">
+        <v>8.9480000000000004</v>
+      </c>
+      <c r="Q17">
+        <v>9.7170000000000005</v>
+      </c>
+      <c r="R17">
+        <v>415</v>
+      </c>
+      <c r="S17">
+        <v>1760</v>
+      </c>
+      <c r="T17">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="U17">
+        <v>1.639</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0.502</v>
+      </c>
+      <c r="Y17">
+        <v>16.818000000000001</v>
+      </c>
+      <c r="Z17">
+        <v>12.5</v>
+      </c>
+      <c r="AA17">
+        <v>18.864000000000001</v>
+      </c>
+      <c r="AB17">
+        <v>2.3860000000000001</v>
+      </c>
+      <c r="AC17">
+        <v>2.8410000000000002</v>
+      </c>
+      <c r="AD17">
+        <v>24.096</v>
+      </c>
+      <c r="AE17">
+        <v>10.843</v>
+      </c>
+      <c r="AF17">
+        <v>40.963999999999999</v>
+      </c>
+      <c r="AG17">
+        <v>7.2290000000000001</v>
+      </c>
+      <c r="AH17">
+        <v>10.542</v>
+      </c>
+      <c r="AI17">
+        <v>7.1589999999999998</v>
+      </c>
+      <c r="AJ17">
+        <v>3.4660000000000002</v>
+      </c>
+      <c r="AK17">
+        <v>7.2160000000000002</v>
+      </c>
+      <c r="AL17">
+        <v>2.1019999999999999</v>
+      </c>
+      <c r="AM17">
+        <v>8.4090000000000007</v>
+      </c>
+      <c r="AN17">
+        <v>15.398</v>
+      </c>
+      <c r="AO17">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="AP17">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="AQ17">
+        <v>816</v>
+      </c>
+      <c r="AR17">
+        <v>923</v>
+      </c>
+      <c r="AS17">
+        <v>18</v>
+      </c>
+      <c r="AT17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" ht="15" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>84</v>
+      </c>
+      <c r="O18">
+        <v>84</v>
+      </c>
+      <c r="P18">
+        <v>8.452</v>
+      </c>
+      <c r="Q18">
+        <v>9.0709999999999997</v>
+      </c>
+      <c r="R18">
+        <v>273</v>
+      </c>
+      <c r="S18">
+        <v>736</v>
+      </c>
+      <c r="T18">
+        <v>0.371</v>
+      </c>
+      <c r="U18">
+        <v>1.583</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="Y18">
+        <v>19.158000000000001</v>
+      </c>
+      <c r="Z18">
+        <v>12.057</v>
+      </c>
+      <c r="AA18">
+        <v>18.885999999999999</v>
+      </c>
+      <c r="AB18">
+        <v>2.5819999999999999</v>
+      </c>
+      <c r="AC18">
+        <v>2.9889999999999999</v>
+      </c>
+      <c r="AD18">
+        <v>23.741</v>
+      </c>
+      <c r="AE18">
+        <v>9.3529999999999998</v>
+      </c>
+      <c r="AF18">
+        <v>27.338000000000001</v>
+      </c>
+      <c r="AG18">
+        <v>12.95</v>
+      </c>
+      <c r="AH18">
+        <v>10.071999999999999</v>
+      </c>
+      <c r="AI18">
+        <v>8.016</v>
+      </c>
+      <c r="AJ18">
+        <v>3.5329999999999999</v>
+      </c>
+      <c r="AK18">
+        <v>6.9290000000000003</v>
+      </c>
+      <c r="AL18">
+        <v>1.087</v>
+      </c>
+      <c r="AM18">
+        <v>10.734</v>
+      </c>
+      <c r="AN18">
+        <v>11.821</v>
+      </c>
+      <c r="AO18">
+        <v>1.014</v>
+      </c>
+      <c r="AP18">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="AQ18">
+        <v>357</v>
+      </c>
+      <c r="AR18">
+        <v>363</v>
+      </c>
+      <c r="AS18">
+        <v>8</v>
+      </c>
+      <c r="AT18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" ht="15" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>106</v>
+      </c>
+      <c r="O19">
+        <v>106</v>
+      </c>
+      <c r="P19">
+        <v>11.16</v>
+      </c>
+      <c r="Q19">
+        <v>12.132</v>
+      </c>
+      <c r="R19">
+        <v>324</v>
+      </c>
+      <c r="S19">
+        <v>1201</v>
+      </c>
+      <c r="T19">
+        <v>0.27</v>
+      </c>
+      <c r="U19">
+        <v>1.7450000000000001</v>
+      </c>
+      <c r="V19">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="Y19">
+        <v>17.484999999999999</v>
+      </c>
+      <c r="Z19">
+        <v>12.856999999999999</v>
+      </c>
+      <c r="AA19">
+        <v>17.068999999999999</v>
+      </c>
+      <c r="AB19">
+        <v>1.7490000000000001</v>
+      </c>
+      <c r="AC19">
+        <v>2.0819999999999999</v>
+      </c>
+      <c r="AD19">
+        <v>2.927</v>
+      </c>
+      <c r="AE19">
+        <v>14.634</v>
+      </c>
+      <c r="AF19">
+        <v>57.073</v>
+      </c>
+      <c r="AG19">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="AH19">
+        <v>17.073</v>
+      </c>
+      <c r="AI19">
+        <v>8.41</v>
+      </c>
+      <c r="AJ19">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="AK19">
+        <v>8.9090000000000007</v>
+      </c>
+      <c r="AL19">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="AM19">
+        <v>8.9090000000000007</v>
+      </c>
+      <c r="AN19">
+        <v>12.49</v>
+      </c>
+      <c r="AO19">
+        <v>1.024</v>
+      </c>
+      <c r="AP19">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="AQ19">
+        <v>566</v>
+      </c>
+      <c r="AR19">
+        <v>612</v>
+      </c>
+      <c r="AS19">
+        <v>27</v>
+      </c>
+      <c r="AT19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" ht="15" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" t="s">
+        <v>51</v>
+      </c>
+      <c r="L20" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>157</v>
+      </c>
+      <c r="O20">
+        <v>157</v>
+      </c>
+      <c r="P20">
+        <v>10.172000000000001</v>
+      </c>
+      <c r="Q20">
+        <v>11.102</v>
+      </c>
+      <c r="R20">
+        <v>450</v>
+      </c>
+      <c r="S20">
+        <v>1637</v>
+      </c>
+      <c r="T20">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="U20">
+        <v>1.752</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>16</v>
+      </c>
+      <c r="X20">
+        <v>0.496</v>
+      </c>
+      <c r="Y20">
+        <v>17.41</v>
+      </c>
+      <c r="Z20">
+        <v>14.385999999999999</v>
+      </c>
+      <c r="AA20">
+        <v>18.204000000000001</v>
+      </c>
+      <c r="AB20">
+        <v>3.177</v>
+      </c>
+      <c r="AC20">
+        <v>1.649</v>
+      </c>
+      <c r="AD20">
+        <v>23.826000000000001</v>
+      </c>
+      <c r="AE20">
+        <v>17.785</v>
+      </c>
+      <c r="AF20">
+        <v>38.591000000000001</v>
+      </c>
+      <c r="AG20">
+        <v>9.7319999999999993</v>
+      </c>
+      <c r="AH20">
+        <v>16.443000000000001</v>
+      </c>
+      <c r="AI20">
+        <v>8.125</v>
+      </c>
+      <c r="AJ20">
+        <v>4.8869999999999996</v>
+      </c>
+      <c r="AK20">
+        <v>7.88</v>
+      </c>
+      <c r="AL20">
+        <v>2.871</v>
+      </c>
+      <c r="AM20">
+        <v>7.5750000000000002</v>
+      </c>
+      <c r="AN20">
+        <v>13.867000000000001</v>
+      </c>
+      <c r="AO20">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="AP20">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="AQ20">
+        <v>792</v>
+      </c>
+      <c r="AR20">
+        <v>811</v>
+      </c>
+      <c r="AS20">
+        <v>28</v>
+      </c>
+      <c r="AT20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:46" ht="15" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>310</v>
+      </c>
+      <c r="O21">
+        <v>310</v>
+      </c>
+      <c r="P21">
+        <v>8.7579999999999991</v>
+      </c>
+      <c r="Q21">
+        <v>9.452</v>
+      </c>
+      <c r="R21">
+        <v>514</v>
+      </c>
+      <c r="S21">
+        <v>2779</v>
+      </c>
+      <c r="T21">
+        <v>0.185</v>
+      </c>
+      <c r="U21">
+        <v>1.6160000000000001</v>
+      </c>
+      <c r="V21">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0.48</v>
+      </c>
+      <c r="Y21">
+        <v>18.495999999999999</v>
+      </c>
+      <c r="Z21">
+        <v>12.84</v>
+      </c>
+      <c r="AA21">
+        <v>18.675999999999998</v>
+      </c>
+      <c r="AB21">
+        <v>2.339</v>
+      </c>
+      <c r="AC21">
+        <v>2.6269999999999998</v>
+      </c>
+      <c r="AD21">
+        <v>8.6709999999999994</v>
+      </c>
+      <c r="AE21">
+        <v>15.414</v>
+      </c>
+      <c r="AF21">
+        <v>57.225000000000001</v>
+      </c>
+      <c r="AG21">
+        <v>5.78</v>
+      </c>
+      <c r="AH21">
+        <v>9.827</v>
+      </c>
+      <c r="AI21">
+        <v>7.665</v>
+      </c>
+      <c r="AJ21">
+        <v>3.4180000000000001</v>
+      </c>
+      <c r="AK21">
+        <v>5.5780000000000003</v>
+      </c>
+      <c r="AL21">
+        <v>1.4750000000000001</v>
+      </c>
+      <c r="AM21">
+        <v>7.7009999999999996</v>
+      </c>
+      <c r="AN21">
+        <v>15.005000000000001</v>
+      </c>
+      <c r="AO21">
+        <v>0.99</v>
+      </c>
+      <c r="AP21">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="AQ21">
+        <v>1282</v>
+      </c>
+      <c r="AR21">
+        <v>1418</v>
+      </c>
+      <c r="AS21">
+        <v>24</v>
+      </c>
+      <c r="AT21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" ht="15" customHeight="1">
+      <c r="M27" t="s">
         <v>88</v>
       </c>
-      <c r="N13">
+      <c r="N27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",N2:N11)</f>
         <v>127.6</v>
       </c>
-      <c r="O13">
+      <c r="O27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",O2:O11)</f>
         <v>126.8</v>
       </c>
-      <c r="P13">
+      <c r="P27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",P2:P11)</f>
         <v>3.3761999999999999</v>
       </c>
-      <c r="Q13">
+      <c r="Q27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",Q2:Q11)</f>
         <v>3.5160000000000005</v>
       </c>
-      <c r="R13">
+      <c r="R27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",R2:R11)</f>
         <v>116.2</v>
       </c>
-      <c r="S13">
+      <c r="S27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",S2:S11)</f>
         <v>471.8</v>
       </c>
-      <c r="T13">
+      <c r="T27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",T2:T11)</f>
         <v>0.251</v>
       </c>
-      <c r="U13">
+      <c r="U27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",U2:U11)</f>
         <v>0.29299999999999998</v>
       </c>
-      <c r="V13">
+      <c r="V27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",V2:V11)</f>
         <v>5.8657999999999992</v>
       </c>
-      <c r="W13">
+      <c r="W27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",W2:W11)</f>
         <v>54.6</v>
       </c>
-      <c r="X13">
+      <c r="X27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",X2:X11)</f>
         <v>0.25339999999999996</v>
       </c>
-      <c r="Y13">
+      <c r="Y27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",Y2:Y11)</f>
         <v>15.954399999999998</v>
       </c>
-      <c r="Z13">
+      <c r="Z27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",Z2:Z11)</f>
         <v>10.714599999999999</v>
       </c>
-      <c r="AA13">
+      <c r="AA27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AA2:AA11)</f>
         <v>8.9987999999999992</v>
       </c>
-      <c r="AB13">
+      <c r="AB27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AB2:AB11)</f>
         <v>0.57940000000000003</v>
       </c>
-      <c r="AC13">
+      <c r="AC27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AC2:AC11)</f>
         <v>1.034</v>
       </c>
-      <c r="AD13">
+      <c r="AD27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AD2:AD11)</f>
         <v>25.308799999999998</v>
       </c>
-      <c r="AE13">
+      <c r="AE27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AE2:AE11)</f>
         <v>1.1960000000000002</v>
       </c>
-      <c r="AF13">
+      <c r="AF27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AF2:AF11)</f>
         <v>5.0468000000000002</v>
       </c>
-      <c r="AG13">
+      <c r="AG27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AG2:AG11)</f>
         <v>2.6348000000000003</v>
       </c>
-      <c r="AH13">
+      <c r="AH27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AH2:AH11)</f>
         <v>15.526599999999998</v>
       </c>
-      <c r="AI13">
+      <c r="AI27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AI2:AI11)</f>
         <v>0.55579999999999996</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AJ2:AJ11)</f>
         <v>4.6411999999999995</v>
       </c>
-      <c r="AK13">
+      <c r="AK27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AK2:AK11)</f>
         <v>4.0304000000000002</v>
       </c>
-      <c r="AL13">
+      <c r="AL27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AL2:AL11)</f>
         <v>1.5728</v>
       </c>
-      <c r="AM13">
+      <c r="AM27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AM2:AM11)</f>
         <v>5.1929999999999996</v>
       </c>
-      <c r="AN13">
+      <c r="AN27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AN2:AN11)</f>
         <v>5.9698000000000002</v>
       </c>
-      <c r="AO13">
+      <c r="AO27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AO2:AO11)</f>
         <v>3.2902</v>
       </c>
-      <c r="AP13">
+      <c r="AP27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AP2:AP11)</f>
         <v>0.62419999999999998</v>
       </c>
-      <c r="AQ13">
+      <c r="AQ27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AQ2:AQ11)</f>
         <v>176.8</v>
       </c>
-      <c r="AR13">
+      <c r="AR27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AR2:AR11)</f>
         <v>255.8</v>
       </c>
-      <c r="AS13">
+      <c r="AS27">
         <f>AVERAGEIF($G$2:$G$11,"Broca",AS2:AS11)</f>
         <v>12.6</v>
       </c>
-      <c r="AT13">
+      <c r="AT27">
         <f>SUMIF($G$2:$G$11,"Broca",AT2:AT11)</f>
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M14" t="s">
+    <row r="28" spans="1:46" ht="15" customHeight="1">
+      <c r="M28" t="s">
         <v>87</v>
       </c>
-      <c r="N14">
+      <c r="N28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", N2:N11)</f>
         <v>245.8</v>
       </c>
-      <c r="O14">
+      <c r="O28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", O2:O11)</f>
         <v>241.2</v>
       </c>
-      <c r="P14">
+      <c r="P28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", P2:P11)</f>
         <v>7.1261999999999999</v>
       </c>
-      <c r="Q14">
+      <c r="Q28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", Q2:Q11)</f>
         <v>7.7152000000000003</v>
       </c>
-      <c r="R14">
+      <c r="R28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", R2:R11)</f>
         <v>246.6</v>
       </c>
-      <c r="S14">
+      <c r="S28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", S2:S11)</f>
         <v>1686.4</v>
       </c>
-      <c r="T14">
+      <c r="T28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", T2:T11)</f>
         <v>0.15140000000000001</v>
       </c>
-      <c r="U14">
+      <c r="U28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", U2:U11)</f>
         <v>1.1792</v>
       </c>
-      <c r="V14">
+      <c r="V28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", V2:V11)</f>
         <v>3.8645999999999994</v>
       </c>
-      <c r="W14">
+      <c r="W28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", W2:W11)</f>
         <v>76.400000000000006</v>
       </c>
-      <c r="X14">
+      <c r="X28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", X2:X11)</f>
         <v>0.39039999999999997</v>
       </c>
-      <c r="Y14">
+      <c r="Y28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", Y2:Y11)</f>
         <v>8.8979999999999997</v>
       </c>
-      <c r="Z14">
+      <c r="Z28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", Z2:Z11)</f>
         <v>23.019799999999996</v>
       </c>
-      <c r="AA14">
+      <c r="AA28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AA2:AA11)</f>
         <v>16.685200000000002</v>
       </c>
-      <c r="AB14">
+      <c r="AB28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AB2:AB11)</f>
         <v>2.8502000000000001</v>
       </c>
-      <c r="AC14">
+      <c r="AC28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AC2:AC11)</f>
         <v>2.9543999999999997</v>
       </c>
-      <c r="AD14">
+      <c r="AD28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AD2:AD11)</f>
         <v>24.341999999999999</v>
       </c>
-      <c r="AE14">
+      <c r="AE28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AE2:AE11)</f>
         <v>7.6912000000000003</v>
       </c>
-      <c r="AF14">
+      <c r="AF28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AF2:AF11)</f>
         <v>21.927799999999998</v>
       </c>
-      <c r="AG14">
+      <c r="AG28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AG2:AG11)</f>
         <v>3.8537999999999997</v>
       </c>
-      <c r="AH14">
+      <c r="AH28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AH2:AH11)</f>
         <v>20.641999999999999</v>
       </c>
-      <c r="AI14">
+      <c r="AI28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AI2:AI11)</f>
         <v>5.4601999999999995</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AJ2:AJ11)</f>
         <v>3.0900000000000003</v>
       </c>
-      <c r="AK14">
+      <c r="AK28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AK2:AK11)</f>
         <v>6.0136000000000003</v>
       </c>
-      <c r="AL14">
+      <c r="AL28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AL2:AL11)</f>
         <v>1.6707999999999998</v>
       </c>
-      <c r="AM14">
+      <c r="AM28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AM2:AM11)</f>
         <v>6.3980000000000006</v>
       </c>
-      <c r="AN14">
+      <c r="AN28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AN2:AN11)</f>
         <v>18.477</v>
       </c>
-      <c r="AO14">
+      <c r="AO28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AO2:AO11)</f>
         <v>0.53900000000000003</v>
       </c>
-      <c r="AP14">
+      <c r="AP28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AP2:AP11)</f>
         <v>0.5643999999999999</v>
       </c>
-      <c r="AQ14">
+      <c r="AQ28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AQ2:AQ11)</f>
         <v>594.4</v>
       </c>
-      <c r="AR14">
+      <c r="AR28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AR2:AR11)</f>
         <v>1026.4000000000001</v>
       </c>
-      <c r="AS14">
+      <c r="AS28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AS2:AS11)</f>
         <v>47.2</v>
       </c>
-      <c r="AT14">
+      <c r="AT28">
         <f>AVERAGEIF($G$2:$G$11,"Wernicke", AT2:AT11)</f>
         <v>55.4</v>
       </c>
     </row>
-    <row r="15" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="M15" t="s">
+    <row r="29" spans="1:46" ht="15" customHeight="1">
+      <c r="M29" t="s">
         <v>89</v>
       </c>
-      <c r="N15">
-        <f>AVERAGEIF($G$2:$G$12,"Generic",N2:N12)</f>
+      <c r="N29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",N2:N21)</f>
         <v>157</v>
       </c>
-      <c r="O15">
-        <f t="shared" ref="O15:AP15" si="0">AVERAGEIF($G$2:$G$12,"Generic",O2:O12)</f>
+      <c r="O29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",O2:O21)</f>
         <v>157</v>
       </c>
-      <c r="P15">
+      <c r="P29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",P2:P12)</f>
+        <v>4.07</v>
+      </c>
+      <c r="Q29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",Q2:Q12)</f>
+        <v>4.3310000000000004</v>
+      </c>
+      <c r="R29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",R2:R12)</f>
+        <v>307</v>
+      </c>
+      <c r="S29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",S2:S12)</f>
+        <v>644</v>
+      </c>
+      <c r="T29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",T2:T12)</f>
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="U29" t="e">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",U2:U12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",V2:V12)</f>
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="W29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",W2:W12)</f>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",X2:X12)</f>
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",Y2:Y12)</f>
+        <v>0.373</v>
+      </c>
+      <c r="Z29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",Z2:Z12)</f>
+        <v>53.726999999999997</v>
+      </c>
+      <c r="AA29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AA2:AA12)</f>
+        <v>3.1789999999999998</v>
+      </c>
+      <c r="AB29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AB2:AB12)</f>
+        <v>15.839</v>
+      </c>
+      <c r="AC29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AC2:AC12)</f>
+        <v>0</v>
+      </c>
+      <c r="AD29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AD2:AD12)</f>
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AE29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AE2:AE12)</f>
+        <v>27.451000000000001</v>
+      </c>
+      <c r="AF29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AF2:AF12)</f>
+        <v>0</v>
+      </c>
+      <c r="AG29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AG2:AG12)</f>
+        <v>14.706</v>
+      </c>
+      <c r="AH29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AH2:AH12)</f>
+        <v>3.9220000000000002</v>
+      </c>
+      <c r="AI29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AI2:AI12)</f>
+        <v>11.765000000000001</v>
+      </c>
+      <c r="AJ29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AJ2:AJ12)</f>
+        <v>4.0369999999999999</v>
+      </c>
+      <c r="AK29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AK2:AK12)</f>
+        <v>5.9009999999999998</v>
+      </c>
+      <c r="AL29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AL2:AL12)</f>
+        <v>7.9189999999999996</v>
+      </c>
+      <c r="AM29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AM2:AM12)</f>
+        <v>0.155</v>
+      </c>
+      <c r="AN29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AN2:AN12)</f>
+        <v>2.0190000000000001</v>
+      </c>
+      <c r="AO29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AO2:AO12)</f>
+        <v>3.8820000000000001</v>
+      </c>
+      <c r="AP29">
+        <f>AVERAGEIF($G$2:$G$12,"Generic",AP2:AP12)</f>
+        <v>3.3919999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" ht="15" customHeight="1">
+      <c r="M30" t="s">
+        <v>107</v>
+      </c>
+      <c r="N30">
+        <f>AVERAGEIF($G$2:$G$21,"Control",N2:N21)</f>
+        <v>161.83333333333334</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ref="O30:AP30" si="0">AVERAGEIF($G$2:$G$21,"Control",O2:O21)</f>
+        <v>161.83333333333334</v>
+      </c>
+      <c r="P30">
+        <f>AVERAGEIF($G$2:$G$21,"Control",P2:P21)</f>
+        <v>9.6994999999999987</v>
+      </c>
+      <c r="Q30">
         <f t="shared" si="0"/>
-        <v>4.07</v>
-      </c>
-      <c r="Q15">
+        <v>10.527499999999998</v>
+      </c>
+      <c r="R30">
         <f t="shared" si="0"/>
-        <v>4.3310000000000004</v>
-      </c>
-      <c r="R15">
+        <v>399.5</v>
+      </c>
+      <c r="S30">
         <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-      <c r="S15">
+        <v>1574.5</v>
+      </c>
+      <c r="T30">
         <f t="shared" si="0"/>
-        <v>644</v>
-      </c>
-      <c r="T15">
+        <v>0.27550000000000002</v>
+      </c>
+      <c r="U30">
         <f t="shared" si="0"/>
-        <v>0.47699999999999998</v>
-      </c>
-      <c r="U15" t="e">
+        <v>1.6696666666666669</v>
+      </c>
+      <c r="V30">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V15">
+        <v>4.5666666666666668E-2</v>
+      </c>
+      <c r="W30">
         <f t="shared" si="0"/>
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="W15">
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="X30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X15">
+        <v>0.49516666666666659</v>
+      </c>
+      <c r="Y30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y15">
+        <v>18.205333333333332</v>
+      </c>
+      <c r="Z30">
         <f t="shared" si="0"/>
-        <v>0.373</v>
-      </c>
-      <c r="Z15">
+        <v>13.163333333333334</v>
+      </c>
+      <c r="AA30">
         <f t="shared" si="0"/>
-        <v>53.726999999999997</v>
-      </c>
-      <c r="AA15">
+        <v>18.131666666666668</v>
+      </c>
+      <c r="AB30">
         <f t="shared" si="0"/>
-        <v>3.1789999999999998</v>
-      </c>
-      <c r="AB15">
+        <v>2.5011666666666668</v>
+      </c>
+      <c r="AC30">
         <f t="shared" si="0"/>
-        <v>15.839</v>
-      </c>
-      <c r="AC15">
+        <v>2.218666666666667</v>
+      </c>
+      <c r="AD30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD15">
+        <v>17.897333333333336</v>
+      </c>
+      <c r="AE30">
         <f t="shared" si="0"/>
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="AE15">
+        <v>12.361499999999999</v>
+      </c>
+      <c r="AF30">
         <f t="shared" si="0"/>
-        <v>27.451000000000001</v>
-      </c>
-      <c r="AF15">
+        <v>42.786166666666674</v>
+      </c>
+      <c r="AG30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG15">
+        <v>8.7270000000000003</v>
+      </c>
+      <c r="AH30">
         <f t="shared" si="0"/>
-        <v>14.706</v>
-      </c>
-      <c r="AH15">
+        <v>13.071833333333332</v>
+      </c>
+      <c r="AI30">
         <f t="shared" si="0"/>
-        <v>3.9220000000000002</v>
-      </c>
-      <c r="AI15">
+        <v>7.9243333333333332</v>
+      </c>
+      <c r="AJ30">
         <f t="shared" si="0"/>
-        <v>11.765000000000001</v>
-      </c>
-      <c r="AJ15">
+        <v>4.0108333333333333</v>
+      </c>
+      <c r="AK30">
         <f t="shared" si="0"/>
-        <v>4.0369999999999999</v>
-      </c>
-      <c r="AK15">
+        <v>7.0473333333333343</v>
+      </c>
+      <c r="AL30">
         <f t="shared" si="0"/>
-        <v>5.9009999999999998</v>
-      </c>
-      <c r="AL15">
+        <v>1.6234999999999999</v>
+      </c>
+      <c r="AM30">
         <f t="shared" si="0"/>
-        <v>7.9189999999999996</v>
-      </c>
-      <c r="AM15">
+        <v>9.0205000000000002</v>
+      </c>
+      <c r="AN30">
         <f t="shared" si="0"/>
-        <v>0.155</v>
-      </c>
-      <c r="AN15">
+        <v>13.341666666666667</v>
+      </c>
+      <c r="AO30">
         <f t="shared" si="0"/>
-        <v>2.0190000000000001</v>
-      </c>
-      <c r="AO15">
+        <v>1.0063333333333333</v>
+      </c>
+      <c r="AP30">
         <f t="shared" si="0"/>
-        <v>3.8820000000000001</v>
-      </c>
-      <c r="AP15">
-        <f t="shared" si="0"/>
-        <v>3.3919999999999999</v>
+        <v>0.93433333333333346</v>
       </c>
     </row>
   </sheetData>
@@ -5785,6 +5674,7 @@
       <sortCondition ref="G1:G11"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>